<commit_message>
migratie documentatie naar gitbook
</commit_message>
<xml_diff>
--- a/integratie/mqtt-berichten.xlsx
+++ b/integratie/mqtt-berichten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijnhendriks/Documents/Arduino/DSMR-API-V2/integratie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijn/Documents/Arduino/DSMR-API-V2/integratie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17FDB38-8C52-4744-8931-140102CD0451}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AB363-C1A3-B24E-90D6-AF0F9A5EBB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15500" xr2:uid="{19021FB8-B14C-EC42-9818-C0A0BF530E25}"/>
   </bookViews>
@@ -87,72 +87,6 @@
     <t>payload</t>
   </si>
   <si>
-    <t>DSMR-API/identification</t>
-  </si>
-  <si>
-    <t>DSMR-API/equipment_id65]</t>
-  </si>
-  <si>
-    <t>DSMR-API/p1_version</t>
-  </si>
-  <si>
-    <t>DSMR-API/timestamp</t>
-  </si>
-  <si>
-    <t>DSMR-API/electricity_tariff</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_delivered</t>
-  </si>
-  <si>
-    <t>DSMR-API/gas_device_type</t>
-  </si>
-  <si>
-    <t>DSMR-API/gas_equipment_id</t>
-  </si>
-  <si>
-    <t>DSMR-API/voltage_l1</t>
-  </si>
-  <si>
-    <t>DSMR-API/current_l1</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_delivered_l1</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_returned_l1</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_returned</t>
-  </si>
-  <si>
-    <t>DSMR-API/energy_delivered_tariff1</t>
-  </si>
-  <si>
-    <t>DSMR-API/energy_delivered_tariff2</t>
-  </si>
-  <si>
-    <t>DSMR-API/energy_returned_tariff1</t>
-  </si>
-  <si>
-    <t>DSMR-API/energy_returned_tariff2</t>
-  </si>
-  <si>
-    <t>DSMR-API/gas_delivered</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_delivered_l2</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_returned_l2</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_delivered_l3</t>
-  </si>
-  <si>
-    <t>DSMR-API/power_returned_l3</t>
-  </si>
-  <si>
     <t>{power_delivered_l2":[{"value":0.703,"unit":"kW"}]}"</t>
   </si>
   <si>
@@ -165,18 +99,6 @@
     <t>{power_returned_l3":[{"value":0,"unit":"kW"}]}"</t>
   </si>
   <si>
-    <t>DSMR-API/voltage_l2</t>
-  </si>
-  <si>
-    <t>DSMR-API/current_l2</t>
-  </si>
-  <si>
-    <t>DSMR-API/voltage_l3</t>
-  </si>
-  <si>
-    <t>DSMR-API/current_l3</t>
-  </si>
-  <si>
     <t>{voltage_l3":[{"value":231,"unit":"V"}]}"</t>
   </si>
   <si>
@@ -190,6 +112,84 @@
   </si>
   <si>
     <t>DSMR = default hostname (aanpassen aan je eigen hostname indien je deze zelf hebt ingesteld)</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/identification</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/p1_version</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/timestamp</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/equipment_id65]</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/energy_delivered_tariff1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/energy_delivered_tariff2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/energy_returned_tariff1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/energy_returned_tariff2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/electricity_tariff</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_delivered</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_returned</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/voltage_l1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/current_l1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/voltage_l2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/current_l2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/voltage_l3</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/current_l3</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_delivered_l1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_returned_l1</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_delivered_l2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_returned_l2</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_delivered_l3</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/power_returned_l3</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/gas_device_type</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/gas_equipment_id</t>
+  </si>
+  <si>
+    <t>TOP TOPIC/gas_delivered</t>
   </si>
 </sst>
 </file>
@@ -544,13 +544,13 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -667,39 +667,39 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -715,39 +715,39 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>